<commit_message>
ECOM90025 and ECOM9004 study materials
</commit_message>
<xml_diff>
--- a/2025/S2/ECOM90025/ADA mark theorycrafting.xlsx
+++ b/2025/S2/ECOM90025/ADA mark theorycrafting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshc\Documents\git\mae_unimelb\2025\S2\ECOM90025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8162A32B-70B9-464D-BFFD-A14F28088808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E955BA-765C-4691-8834-980E68961E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{0B5E8DD2-158E-4F4C-8AD5-DD83C891B8D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0B5E8DD2-158E-4F4C-8AD5-DD83C891B8D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Assignments</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Final mark</t>
+  </si>
+  <si>
+    <t>Presentation</t>
   </si>
 </sst>
 </file>
@@ -466,18 +469,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0213C5F1-5603-4ED5-BC99-E2FCA27ED91B}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -485,7 +488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,10 +497,10 @@
         <v>78.75</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -506,7 +509,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -515,7 +518,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -524,7 +527,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -533,7 +536,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -542,146 +545,157 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <f>AVERAGE(B10:B19)*100</f>
+      <c r="B11">
+        <f>AVERAGE(B12:B21)*100</f>
         <v>58.333333333333336</v>
       </c>
-      <c r="C9">
+      <c r="C11">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <f>3/3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <f>2.5/3</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>4</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>5</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <f>0</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>6</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>7</v>
       </c>
-      <c r="B16">
+      <c r="B18">
         <f>2.5/3</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>8</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <f>2.5/3</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>9</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <f>3/3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B21">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B21">
+      <c r="B23">
         <v>100</v>
       </c>
-      <c r="C21">
+      <c r="C23">
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>50</v>
       </c>
-      <c r="C22">
+      <c r="C24">
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C23">
+      <c r="C25">
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="3">
-        <f>B2*C2+B9*C9+B21*C21+B22*C22+B23*C23</f>
-        <v>55.291666666666671</v>
+      <c r="C27" s="3">
+        <f>B2*C2+B11*C11+B23*C23+B24*C24+B25*C25+B9*C9</f>
+        <v>53.416666666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>